<commit_message>
exp list update + train script
</commit_message>
<xml_diff>
--- a/DynEnv/examples/experiments_bookkeeping.xlsx
+++ b/DynEnv/examples/experiments_bookkeeping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpatr\Documents\GitHub\DynEnv\DynEnv\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8645CE72-5BD6-42A4-AC5A-5B83C31D66EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F8803C-7A0A-4DD7-A886-5CF90FE3B87E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0DEC3E77-3EB3-4C71-BF44-3494F42E096B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Experiments!$B$1:$U$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Experiments!$B$1:$U$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Observation</t>
   </si>
@@ -198,19 +198,19 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -525,11 +525,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A700E75-B385-4CEA-9500-152092F9C6D8}">
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,34 +622,34 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="6" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="3" t="s">
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -667,178 +667,49 @@
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
       <c r="P4">
-        <f t="shared" ref="P4:P18" si="0">IF(ISBLANK(C4),0,0.01)</f>
+        <f t="shared" ref="P4:P7" si="0">IF(ISBLANK(C4),0,0.01)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P5">
-        <f t="shared" si="0"/>
+        <f>IF(ISBLANK(C5),0,0.01)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
         <v>25</v>
       </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
       <c r="P6">
         <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
         <v>25</v>
       </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
       <c r="P7">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" t="s">
-        <v>25</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" t="s">
-        <v>25</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>24</v>
-      </c>
-      <c r="P17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" t="s">
-        <v>25</v>
-      </c>
-      <c r="P18">
         <f t="shared" si="0"/>
         <v>0.01</v>
       </c>

</xml_diff>